<commit_message>
excel file for kolich
</commit_message>
<xml_diff>
--- a/resdataASW_all_m3.xlsx
+++ b/resdataASW_all_m3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OparinMV\Documents\GitHub\GZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD6E9CC-079A-4E51-8F27-2A85CC5DE97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDD8B9C-2F8F-44E7-877F-2E3DEBB2C470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="140m3" sheetId="1" r:id="rId1"/>
@@ -7551,8 +7551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7744,10 +7744,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7800,6 +7800,11 @@
       </c>
       <c r="P1" s="16" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>